<commit_message>
PDF con capturas y primera forma normal
</commit_message>
<xml_diff>
--- a/ER Santiago Ramirez Arenas/Normalizacion.xlsx
+++ b/ER Santiago Ramirez Arenas/Normalizacion.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\C1-2023-QA-BD-02\ER Santiago Ramirez Arenas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D9B809-CC44-4C71-9516-6286149D808A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1737A5-9D9A-47CD-AF21-D1631F8CA389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{D3FD2DD2-1160-4627-B730-241ECCC7FE6A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{D3FD2DD2-1160-4627-B730-241ECCC7FE6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Registro tablas " sheetId="3" r:id="rId1"/>
-    <sheet name="Normalizacion" sheetId="1" r:id="rId2"/>
-    <sheet name="Primera forma normal" sheetId="2" r:id="rId3"/>
+    <sheet name="Primera forma normal 1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="59">
   <si>
     <t>Orden de servicio</t>
   </si>
@@ -185,13 +184,43 @@
   </si>
   <si>
     <t>Premium</t>
+  </si>
+  <si>
+    <t>Segundo Nombre</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pepito </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segundo nombre </t>
+  </si>
+  <si>
+    <t>Son</t>
+  </si>
+  <si>
+    <t>Goku</t>
+  </si>
+  <si>
+    <t>Numero de identificacion Operador</t>
+  </si>
+  <si>
+    <t>Tipo de seccional</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,8 +228,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,6 +297,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -283,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -298,7 +346,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -313,6 +360,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D3B447-BFB4-47CB-8579-B1DAE19137C4}">
   <dimension ref="B3:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="37" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,14 +701,14 @@
         <v>0</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="H3" s="10" t="s">
+      <c r="F3" s="7"/>
+      <c r="H3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="10"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -670,7 +723,7 @@
       <c r="F4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="1">
@@ -690,7 +743,7 @@
       <c r="F5" s="4">
         <v>1</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -710,7 +763,7 @@
       <c r="F6" s="4">
         <v>12</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I6" s="1">
@@ -724,7 +777,7 @@
       <c r="C7" s="1">
         <v>1004776990</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -732,7 +785,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -740,7 +793,7 @@
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -752,11 +805,11 @@
         <v>6</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="H10" s="6" t="s">
+      <c r="F10" s="8"/>
+      <c r="H10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="I10" s="1">
@@ -764,19 +817,19 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1">
         <v>29</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="1">
         <v>40</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="I11" s="1">
@@ -784,13 +837,13 @@
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -798,13 +851,13 @@
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="1">
         <v>313826242</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="1">
@@ -812,31 +865,31 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="12"/>
+      <c r="I14" s="11"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -850,13 +903,13 @@
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="1">
         <v>14</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -870,13 +923,13 @@
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F17" s="1">
@@ -890,13 +943,13 @@
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="1">
         <v>1004776990</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F18" s="1">
@@ -910,7 +963,7 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="1">
@@ -918,17 +971,17 @@
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="E22" s="11" t="s">
+      <c r="C22" s="6"/>
+      <c r="E22" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="11"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="1">
@@ -942,7 +995,7 @@
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -956,7 +1009,7 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="1">
@@ -964,7 +1017,7 @@
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -972,7 +1025,7 @@
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -980,7 +1033,7 @@
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -988,7 +1041,7 @@
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -996,7 +1049,7 @@
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="1">
@@ -1004,7 +1057,7 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C31" s="1">
@@ -1018,26 +1071,327 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FE1D43-BB1C-4858-B1D0-57845AFFA3FE}">
-  <dimension ref="A1"/>
+  <dimension ref="C3:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082B992F-4600-4536-BBCF-0EDF84F04728}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="30.85546875" customWidth="1"/>
+    <col min="10" max="10" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>36903</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1004776990</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="1">
+        <v>313826242</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1004776990</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="F24" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1">
+        <v>18</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="1">
+        <v>10047982234</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="1">
+        <v>882921886</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="1">
+        <v>10047982234</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="1">
+        <v>30303993</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" s="1">
+        <v>10298222</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>